<commit_message>
make player and viewport move
</commit_message>
<xml_diff>
--- a/src/applications/sushkevich/map.xlsx
+++ b/src/applications/sushkevich/map.xlsx
@@ -793,7 +793,7 @@
   <dimension ref="A1:Z101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,7 +1113,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="41">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
       <c r="B10" s="29"/>
@@ -1206,7 +1206,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="7">
         <v>11</v>
       </c>
       <c r="B13" s="11"/>
@@ -1237,7 +1237,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="7">
         <v>12</v>
       </c>
       <c r="B14" s="17"/>
@@ -1262,7 +1262,7 @@
       <c r="U14" s="34"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="7">
         <v>13</v>
       </c>
       <c r="B15" s="15"/>
@@ -1290,7 +1290,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="41">
         <v>14</v>
       </c>
       <c r="B16" s="15"/>

</xml_diff>